<commit_message>
keep text input in colorization, check Vietnamese spell in BangChu
</commit_message>
<xml_diff>
--- a/TestFiles/NumberInTextTest.xlsx
+++ b/TestFiles/NumberInTextTest.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\GR2\MyExcelAddin\TestFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8FEB0EC6-D970-46F7-A797-E26F3F8A0832}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{080D4E82-C74F-46D2-97CE-173A12E9478B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3360" yWindow="2100" windowWidth="17280" windowHeight="9984" xr2:uid="{0C2B33B1-6452-4974-8B12-5857E33D7479}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{0C2B33B1-6452-4974-8B12-5857E33D7479}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -54,9 +54,20 @@
 </metadata>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
+  <si>
+    <t>But held</t>
+  </si>
+  <si>
+    <t>And high</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -64,13 +75,39 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF0F0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -85,9 +122,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -402,10 +441,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{631260F7-DFAE-4E2E-8CD1-FC05088DCB14}">
-  <dimension ref="A1:C29"/>
+  <dimension ref="A1:C45"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B32" sqref="B32"/>
+    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
+      <selection activeCell="B27" sqref="B27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -421,336 +460,402 @@
         <v/>
       </c>
     </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C2" t="str" cm="1">
+        <f t="array" ref="C2">_xll.BangChu(A2)</f>
+        <v/>
+      </c>
+    </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>1</v>
+      </c>
+      <c r="B3" t="str" cm="1">
+        <f t="array" ref="B3">_xll.InText(A3)</f>
+        <v>One</v>
+      </c>
       <c r="C3" t="str" cm="1">
         <f t="array" ref="C3">_xll.BangChu(A3)</f>
-        <v/>
+        <v>Một</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4">
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="B4" t="str" cm="1">
         <f t="array" ref="B4">_xll.InText(A4)</f>
-        <v>One</v>
+        <v>Twelve</v>
       </c>
       <c r="C4" t="str" cm="1">
         <f t="array" ref="C4">_xll.BangChu(A4)</f>
-        <v>Một</v>
+        <v>Mười hai</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5">
-        <v>12</v>
+        <v>123</v>
       </c>
       <c r="B5" t="str" cm="1">
         <f t="array" ref="B5">_xll.InText(A5)</f>
-        <v>Twelve</v>
+        <v>One hundred twenty-three</v>
       </c>
       <c r="C5" t="str" cm="1">
         <f t="array" ref="C5">_xll.BangChu(A5)</f>
-        <v>Mười hai</v>
+        <v>Một trăm hai mươi ba</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6">
-        <v>123</v>
+        <v>1234</v>
       </c>
       <c r="B6" t="str" cm="1">
         <f t="array" ref="B6">_xll.InText(A6)</f>
-        <v>One hundred twenty-three</v>
+        <v>One thousand, two hundred thirty-four</v>
       </c>
       <c r="C6" t="str" cm="1">
         <f t="array" ref="C6">_xll.BangChu(A6)</f>
-        <v>Một trăm hai mươi ba</v>
+        <v>Một nghìn, hai trăm ba mươi bốn</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7">
-        <v>1234</v>
+        <v>12345</v>
       </c>
       <c r="B7" t="str" cm="1">
         <f t="array" ref="B7">_xll.InText(A7)</f>
-        <v>One thousand, two hundred thirty-four</v>
+        <v>Twelve thousand, three hundred forty-five</v>
       </c>
       <c r="C7" t="str" cm="1">
         <f t="array" ref="C7">_xll.BangChu(A7)</f>
-        <v>Một nghìn, hai trăm ba mươi bốn</v>
+        <v>Mười hai nghìn, ba trăm bốn mươi lăm</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8">
-        <v>12345</v>
+        <v>123456</v>
       </c>
       <c r="B8" t="str" cm="1">
         <f t="array" ref="B8">_xll.InText(A8)</f>
-        <v>Twelve thousand, three hundred forty-five</v>
+        <v>One hundred twenty-three thousand, four hundred fifty-six</v>
       </c>
       <c r="C8" t="str" cm="1">
         <f t="array" ref="C8">_xll.BangChu(A8)</f>
-        <v>Mười hai nghìn, ba trăm bốn mươi lăm</v>
+        <v>Một trăm hai mươi ba nghìn, bốn trăm năm mươi sáu</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9">
-        <v>123456</v>
+        <v>1234567</v>
       </c>
       <c r="B9" t="str" cm="1">
         <f t="array" ref="B9">_xll.InText(A9)</f>
-        <v>One hundred twenty-three thousand, four hundred fifty-six</v>
+        <v>One million, two hundred thirty-four thousand, five hundred sixty-seven</v>
       </c>
       <c r="C9" t="str" cm="1">
         <f t="array" ref="C9">_xll.BangChu(A9)</f>
-        <v>Một trăm hai mươi ba nghìn, bốn trăm năm mươi sáu</v>
+        <v>Một triệu, hai trăm ba mươi bốn nghìn, năm trăm sáu mươi bẩy</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10">
-        <v>1234567</v>
+        <v>12345678</v>
       </c>
       <c r="B10" t="str" cm="1">
         <f t="array" ref="B10">_xll.InText(A10)</f>
-        <v>One million, two hundred thirty-four thousand, five hundred sixty-seven</v>
+        <v>Twelve million, three hundred forty-five thousand, six hundred seventy-eight</v>
       </c>
       <c r="C10" t="str" cm="1">
         <f t="array" ref="C10">_xll.BangChu(A10)</f>
-        <v>Một triệu, hai trăm ba mươi bốn nghìn, năm trăm sáu mươi bẩy</v>
+        <v>Mười hai triệu, ba trăm bốn mươi lăm nghìn, sáu trăm bẩy mươi tám</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A11">
-        <v>12345678</v>
-      </c>
       <c r="B11" t="str" cm="1">
         <f t="array" ref="B11">_xll.InText(A11)</f>
-        <v>Twelve million, three hundred forty-five thousand, six hundred seventy-eight</v>
+        <v/>
       </c>
       <c r="C11" t="str" cm="1">
         <f t="array" ref="C11">_xll.BangChu(A11)</f>
-        <v>Mười hai triệu, ba trăm bốn mươi lăm nghìn, sáu trăm bẩy mươi tám</v>
+        <v/>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>123456789</v>
+      </c>
       <c r="B12" t="str" cm="1">
         <f t="array" ref="B12">_xll.InText(A12)</f>
-        <v/>
+        <v>One hundred twenty-three million, four hundred fifty-six thousand, seven hundred eighty-nine</v>
       </c>
       <c r="C12" t="str" cm="1">
         <f t="array" ref="C12">_xll.BangChu(A12)</f>
-        <v/>
+        <v>Một trăm hai mươi ba triệu, bốn trăm năm mươi sáu nghìn, bẩy trăm tám mươi chín</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13">
-        <v>123456789</v>
+        <v>1234567891</v>
       </c>
       <c r="B13" t="str" cm="1">
         <f t="array" ref="B13">_xll.InText(A13)</f>
-        <v>One hundred twenty-three million, four hundred fifty-six thousand, seven hundred eighty-nine</v>
+        <v>One billion, two hundred thirty-four million, five hundred sixty-seven thousand, eight hundred ninety-one</v>
       </c>
       <c r="C13" t="str" cm="1">
         <f t="array" ref="C13">_xll.BangChu(A13)</f>
-        <v>Một trăm hai mươi ba triệu, bốn trăm năm mươi sáu nghìn, bẩy trăm tám mươi chín</v>
+        <v>Một tỷ, hai trăm ba mươi bốn triệu, năm trăm sáu mươi bẩy nghìn, tám trăm chín mươi mốt</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A14">
-        <v>1234567891</v>
-      </c>
       <c r="B14" t="str" cm="1">
         <f t="array" ref="B14">_xll.InText(A14)</f>
-        <v>One billion, two hundred thirty-four million, five hundred sixty-seven thousand, eight hundred ninety-one</v>
+        <v/>
       </c>
       <c r="C14" t="str" cm="1">
         <f t="array" ref="C14">_xll.BangChu(A14)</f>
-        <v>Một tỷ, hai trăm ba mươi bốn triệu, năm trăm sáu mươi bẩy nghìn, tám trăm chín mươi mốt</v>
+        <v/>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>2147483647</v>
+      </c>
       <c r="B15" t="str" cm="1">
         <f t="array" ref="B15">_xll.InText(A15)</f>
-        <v/>
+        <v>Two billion, one hundred forty-seven million, four hundred eighty-three thousand, six hundred forty-seven</v>
       </c>
       <c r="C15" t="str" cm="1">
         <f t="array" ref="C15">_xll.BangChu(A15)</f>
-        <v/>
+        <v>Hai tỷ, một trăm bốn mươi bẩy triệu, bốn trăm tám mươi ba nghìn, sáu trăm bốn mươi bẩy</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16">
-        <v>2147483647</v>
+        <v>2147483648</v>
       </c>
       <c r="B16" t="str" cm="1">
         <f t="array" ref="B16">_xll.InText(A16)</f>
-        <v>Two billion, one hundred forty-seven million, four hundred eighty-three thousand, six hundred forty-seven</v>
+        <v>Two billion, one hundred forty-seven million, four hundred eighty-three thousand, six hundred forty-eight</v>
       </c>
       <c r="C16" t="str" cm="1">
         <f t="array" ref="C16">_xll.BangChu(A16)</f>
-        <v>Hai tỷ, một trăm bốn mươi bẩy triệu, bốn trăm tám mươi ba nghìn, sáu trăm bốn mươi bẩy</v>
+        <v>Hai tỷ, một trăm bốn mươi bẩy triệu, bốn trăm tám mươi ba nghìn, sáu trăm bốn mươi tám</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A17">
-        <v>2147483648</v>
-      </c>
       <c r="B17" t="str" cm="1">
         <f t="array" ref="B17">_xll.InText(A17)</f>
-        <v>Two billion, one hundred forty-seven million, four hundred eighty-three thousand, six hundred forty-eight</v>
+        <v/>
       </c>
       <c r="C17" t="str" cm="1">
         <f t="array" ref="C17">_xll.BangChu(A17)</f>
-        <v>Hai tỷ, một trăm bốn mươi bẩy triệu, bốn trăm tám mươi ba nghìn, sáu trăm bốn mươi tám</v>
+        <v/>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>-11</v>
+      </c>
       <c r="B18" t="str" cm="1">
         <f t="array" ref="B18">_xll.InText(A18)</f>
-        <v/>
+        <v>Negative eleven</v>
       </c>
       <c r="C18" t="str" cm="1">
         <f t="array" ref="C18">_xll.BangChu(A18)</f>
-        <v/>
+        <v>Âm mười một</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19">
-        <v>-11</v>
+        <v>12345678912</v>
       </c>
       <c r="B19" t="str" cm="1">
         <f t="array" ref="B19">_xll.InText(A19)</f>
-        <v>Negative eleven</v>
+        <v>Twelve billion, three hundred forty-five million, six hundred seventy-eight thousand, nine hundred twelve</v>
       </c>
       <c r="C19" t="str" cm="1">
         <f t="array" ref="C19">_xll.BangChu(A19)</f>
-        <v>Âm mười một</v>
+        <v>Mười hai tỷ, ba trăm bốn mươi lăm triệu, sáu trăm bẩy mươi tám nghìn, chín trăm mười hai</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20">
-        <v>12345678912</v>
+        <v>10000000000</v>
       </c>
       <c r="B20" t="str" cm="1">
         <f t="array" ref="B20">_xll.InText(A20)</f>
-        <v>Twelve billion, three hundred forty-five million, six hundred seventy-eight thousand, nine hundred twelve</v>
+        <v>Ten billion</v>
       </c>
       <c r="C20" t="str" cm="1">
         <f t="array" ref="C20">_xll.BangChu(A20)</f>
-        <v>Mười hai tỷ, ba trăm bốn mươi lăm triệu, sáu trăm bẩy mươi tám nghìn, chín trăm mười hai</v>
+        <v>Mười tỷ</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21">
-        <v>10000000000</v>
+        <v>9999999999</v>
       </c>
       <c r="B21" t="str" cm="1">
         <f t="array" ref="B21">_xll.InText(A21)</f>
-        <v>Ten billion</v>
+        <v>Nine billion, nine hundred ninety-nine million, nine hundred ninety-nine thousand, nine hundred ninety-nine</v>
       </c>
       <c r="C21" t="str" cm="1">
         <f t="array" ref="C21">_xll.BangChu(A21)</f>
-        <v>Mười tỷ</v>
+        <v>Chín tỷ, chín trăm chín mươi chín triệu, chín trăm chín mươi chín nghìn, chín trăm chín mươi chín</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A22">
-        <v>9999999999</v>
+      <c r="A22" s="1">
+        <v>123456789123</v>
       </c>
       <c r="B22" t="str" cm="1">
         <f t="array" ref="B22">_xll.InText(A22)</f>
-        <v>Nine billion, nine hundred ninety-nine million, nine hundred ninety-nine thousand, nine hundred ninety-nine</v>
+        <v>One hundred twenty-three billion, four hundred fifty-six million, seven hundred eighty-nine thousand, one hundred twenty-three</v>
       </c>
       <c r="C22" t="str" cm="1">
         <f t="array" ref="C22">_xll.BangChu(A22)</f>
-        <v>Chín tỷ, chín trăm chín mươi chín triệu, chín trăm chín mươi chín nghìn, chín trăm chín mươi chín</v>
+        <v>Một trăm hai mươi ba tỷ, bốn trăm năm mươi sáu triệu, bẩy trăm tám mươi chín nghìn, một trăm hai mươi ba</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" s="1">
-        <v>123456789123</v>
+        <v>123456789123456</v>
       </c>
       <c r="B23" t="str" cm="1">
         <f t="array" ref="B23">_xll.InText(A23)</f>
-        <v>One hundred twenty-three billion, four hundred fifty-six million, seven hundred eighty-nine thousand, one hundred twenty-three</v>
+        <v>One hundred twenty-threetrillion, four hundred fifty-six billion, seven hundred eighty-nine million, one hundred twenty-three thousand, four hundred fifty-six</v>
       </c>
       <c r="C23" t="str" cm="1">
         <f t="array" ref="C23">_xll.BangChu(A23)</f>
-        <v>Một trăm hai mươi ba tỷ, bốn trăm năm mươi sáu triệu, bẩy trăm tám mươi chín nghìn, một trăm hai mươi ba</v>
+        <v>Một trăm hai mươi ba nghìn tỷ, bốn trăm năm mươi sáu tỷ, bẩy trăm tám mươi chín triệu, một trăm hai mươi ba nghìn, bốn trăm năm mươi sáu</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" s="1">
-        <v>123456789123456</v>
+        <v>1234567891234560</v>
       </c>
       <c r="B24" t="str" cm="1">
         <f t="array" ref="B24">_xll.InText(A24)</f>
-        <v>One hundred twenty-threetrillion, four hundred fifty-six billion, seven hundred eighty-nine million, one hundred twenty-three thousand, four hundred fifty-six</v>
+        <v>One quadrillion, two hundred thirty-fourtrillion, five hundred sixty-seven billion, eight hundred ninety-one million, two hundred thirty-four thousand, five hundred sixty-zero</v>
       </c>
       <c r="C24" t="str" cm="1">
         <f t="array" ref="C24">_xll.BangChu(A24)</f>
-        <v>Một trăm hai mươi ba nghìn tỷ, bốn trăm năm mươi sáu tỷ, bẩy trăm tám mươi chín triệu, một trăm hai mươi ba nghìn, bốn trăm năm mươi sáu</v>
+        <v>Một triệu tỷ, hai trăm ba mươi bốn nghìn tỷ, năm trăm sáu mươi bẩy tỷ, tám trăm chín mươi mốt triệu, hai trăm ba mươi bốn nghìn, năm trăm sáu mươi</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A25" s="1">
-        <v>1234567891234560</v>
-      </c>
       <c r="B25" t="str" cm="1">
         <f t="array" ref="B25">_xll.InText(A25)</f>
-        <v>One quadrillion, two hundred thirty-fourtrillion, five hundred sixty-seven billion, eight hundred ninety-one million, two hundred thirty-four thousand, five hundred sixty-zero</v>
+        <v/>
       </c>
       <c r="C25" t="str" cm="1">
         <f t="array" ref="C25">_xll.BangChu(A25)</f>
-        <v>Một triệu tỷ, hai trăm ba mươi bốn nghìn tỷ, năm trăm sáu mươi bẩy tỷ, tám trăm chín mươi mốt triệu, hai trăm ba mươi bốn nghìn, năm trăm sáu mươi</v>
+        <v/>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A26" s="1">
+        <v>101100110</v>
+      </c>
       <c r="B26" t="str" cm="1">
         <f t="array" ref="B26">_xll.InText(A26)</f>
-        <v/>
+        <v>One hundred one million, one hundred thousand, one hundred ten</v>
       </c>
       <c r="C26" t="str" cm="1">
         <f t="array" ref="C26">_xll.BangChu(A26)</f>
-        <v/>
+        <v>Một trăm linh một triệu, một trăm nghìn, một trăm mười</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" s="1">
-        <v>101100110</v>
+        <v>110111000</v>
       </c>
       <c r="B27" t="str" cm="1">
         <f t="array" ref="B27">_xll.InText(A27)</f>
-        <v>One hundred one million, one hundred thousand, one hundred ten</v>
+        <v>One hundred ten million, one hundred eleven thousand</v>
       </c>
       <c r="C27" t="str" cm="1">
         <f t="array" ref="C27">_xll.BangChu(A27)</f>
-        <v>Một trăm linh một triệu, một trăm nghìn, một trăm mười</v>
+        <v>Một trăm mười triệu, một trăm mười một nghìn</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28" s="1">
-        <v>110111000</v>
+        <v>111000111</v>
       </c>
       <c r="B28" t="str" cm="1">
         <f t="array" ref="B28">_xll.InText(A28)</f>
-        <v>One hundred ten million, one hundred eleven thousand</v>
+        <v>One hundred eleven million, one hundred eleven</v>
       </c>
       <c r="C28" t="str" cm="1">
         <f t="array" ref="C28">_xll.BangChu(A28)</f>
-        <v>Một trăm mười triệu, một trăm mười một nghìn</v>
+        <v>Một trăm mười một triệu, một trăm mười một</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29" s="1">
-        <v>111000111</v>
-      </c>
-      <c r="B29" t="str" cm="1">
+        <v>108011</v>
+      </c>
+      <c r="B29" s="3" t="str" cm="1">
         <f t="array" ref="B29">_xll.InText(A29)</f>
-        <v>One hundred eleven million, one hundred eleven</v>
+        <v>One hundred eight thousand,  eleven</v>
       </c>
       <c r="C29" t="str" cm="1">
         <f t="array" ref="C29">_xll.BangChu(A29)</f>
-        <v>Một trăm mười một triệu, một trăm mười một</v>
+        <v>Một trăm linh tám nghìn, không trăm mười một</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A30" s="1">
+        <v>108001</v>
+      </c>
+      <c r="B30" s="3" t="str" cm="1">
+        <f t="array" ref="B30">_xll.InText(A30)</f>
+        <v>One hundred eight thousand,  one</v>
+      </c>
+      <c r="C30" t="str" cm="1">
+        <f t="array" ref="C30">_xll.BangChu(A30)</f>
+        <v>Một trăm linh tám nghìn, không trăm linh một</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B31" s="2">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B32" s="2">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="33" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B33" s="2">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="34" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B34" s="2">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="35" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B35" s="2">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="39" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B39" s="2">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="42" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B42" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="45" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B45" t="s">
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>